<commit_message>
EPBDS-12754 United Spreadsheet Result type contains full steps name like row_columns
</commit_message>
<xml_diff>
--- a/STUDIO/org.openl.rules.test/test-resources/functionality/EPBDS-8059_Not_very_big_Spreadsheet/Main.xlsx
+++ b/STUDIO/org.openl.rules.test/test-resources/functionality/EPBDS-8059_Not_very_big_Spreadsheet/Main.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25028"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\openl-tablets\STUDIO\org.openl.rules.test\test-resources\functionality\EPBDS-8059_Not_very_big_Spreadsheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3DD45AB-18EA-496B-9A16-6E4F34BE9B40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DAB81A8-187A-444A-A9F9-73C40DD805A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4930" yWindow="1120" windowWidth="28390" windowHeight="14230" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="15630" yWindow="3420" windowWidth="18460" windowHeight="15550" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Rules" sheetId="5" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4661" uniqueCount="659">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4659" uniqueCount="660">
   <si>
     <t>Steps</t>
   </si>
@@ -2009,7 +2009,10 @@
     <t>StepZ</t>
   </si>
   <si>
-    <t>_res_["Value1_Step2"] : Double</t>
+    <t>_res_["Step1"] : Double</t>
+  </si>
+  <si>
+    <t>_res_["Step2"] : Double</t>
   </si>
 </sst>
 </file>
@@ -2422,8 +2425,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:T64"/>
   <sheetViews>
-    <sheetView topLeftCell="A27" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A49" sqref="A49:XFD49"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A33" sqref="A33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5"/>
@@ -17111,10 +17114,14 @@
   <dimension ref="A2:G27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L13" sqref="L13"/>
+      <selection activeCell="L17" sqref="L17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5"/>
+  <cols>
+    <col min="4" max="4" width="23" customWidth="1"/>
+    <col min="5" max="5" width="14.26953125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="2" spans="2:4" s="11" customFormat="1"/>
     <row r="3" spans="2:4" s="11" customFormat="1">
@@ -17272,14 +17279,12 @@
         <v>111</v>
       </c>
       <c r="D24" s="11" t="s">
-        <v>129</v>
+        <v>658</v>
       </c>
       <c r="E24" s="11" t="s">
-        <v>658</v>
-      </c>
-      <c r="F24" s="11" t="s">
-        <v>130</v>
-      </c>
+        <v>659</v>
+      </c>
+      <c r="F24" s="11"/>
       <c r="G24" s="11"/>
     </row>
     <row r="25" spans="1:7">
@@ -17296,9 +17301,7 @@
       <c r="E25" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="F25" s="11" t="s">
-        <v>36</v>
-      </c>
+      <c r="F25" s="11"/>
       <c r="G25" s="11"/>
     </row>
     <row r="26" spans="1:7">
@@ -17327,10 +17330,10 @@
         <v>109</v>
       </c>
       <c r="D27" s="11"/>
-      <c r="E27" s="11"/>
-      <c r="F27" s="11">
+      <c r="E27" s="11">
         <v>4</v>
       </c>
+      <c r="F27" s="11"/>
       <c r="G27" s="11"/>
     </row>
   </sheetData>
@@ -17343,7 +17346,7 @@
   <dimension ref="A3:J41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C24" sqref="C24:C27"/>
+      <selection activeCell="H28" sqref="H28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5"/>

</xml_diff>